<commit_message>
Se organizan las carpetas en su destino
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,7 +20,7 @@
     <t>Activity Name</t>
   </si>
   <si>
-    <t>2c3200f0-d5b4-4dd4-9f40-43e98b479337</t>
+    <t>1f4c7be5-410a-42c2-a297-a89e99fde061</t>
   </si>
   <si>
     <t>Activity 1</t>
@@ -53,7 +53,7 @@
     <t>44</t>
   </si>
   <si>
-    <t>52bb18aa-376a-4158-8314-f45744c8ec1a</t>
+    <t>c96e1fd1-f92f-422c-b339-dd4223320a26</t>
   </si>
   <si>
     <t>Activity 2</t>
@@ -62,19 +62,19 @@
     <t>Task 1 for Activity 2</t>
   </si>
   <si>
-    <t>30</t>
+    <t>29</t>
   </si>
   <si>
     <t>Task 2 for Activity 2</t>
   </si>
   <si>
-    <t>40</t>
+    <t>39</t>
   </si>
   <si>
     <t>Task 3 for Activity 2</t>
   </si>
   <si>
-    <t>55</t>
+    <t>54</t>
   </si>
 </sst>
 </file>

</xml_diff>